<commit_message>
Planilhas + Exxecuções e tuning A-GEO2real1_P e A-GEO2real2_P_DS_fixo
</commit_message>
<xml_diff>
--- a/ExecucoesGerais/PARAMETROSLIVRES2.xlsx
+++ b/ExecucoesGerais/PARAMETROSLIVRES2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7905"/>
+    <workbookView windowWidth="14460" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="61">
   <si>
     <t>GRIEWANGK</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>interv=</t>
-  </si>
-  <si>
-    <t>std1=</t>
   </si>
   <si>
     <t>tau=</t>
@@ -207,8 +204,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -235,19 +232,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -260,7 +249,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,13 +272,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -297,16 +279,22 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,36 +303,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,21 +317,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,19 +391,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,6 +415,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -436,13 +445,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,13 +499,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,103 +559,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,65 +733,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -817,8 +760,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -833,153 +791,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1513,10 +1510,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:AA83"/>
+  <dimension ref="B1:AA86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="D61" workbookViewId="0">
+      <selection activeCell="T84" sqref="T84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -4827,8 +4824,8 @@
         <v>1000</v>
       </c>
       <c r="M76" s="66"/>
-      <c r="P76" s="67" t="s">
-        <v>55</v>
+      <c r="P76" s="63">
+        <v>1</v>
       </c>
       <c r="Q76" s="69">
         <v>10</v>
@@ -4839,30 +4836,30 @@
     </row>
     <row r="77" spans="7:18">
       <c r="G77" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="H77" s="65">
+        <v>2</v>
+      </c>
+      <c r="M77" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="H77" s="65">
-        <v>2</v>
-      </c>
-      <c r="M77" s="67" t="s">
+      <c r="N77" s="68">
+        <v>10</v>
+      </c>
+      <c r="O77" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="N77" s="68">
-        <v>2</v>
-      </c>
-      <c r="O77" s="69" t="s">
-        <v>58</v>
-      </c>
       <c r="P77" s="63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q77" s="63">
-        <f t="shared" ref="Q77:Q83" si="0">Q76/(P77*$N$77)</f>
-        <v>5</v>
+        <f>Q76/(P76*$N$77)</f>
+        <v>1</v>
       </c>
       <c r="R77" s="63">
-        <f t="shared" ref="R77:R83" si="1">R76/$N$77</f>
-        <v>5</v>
+        <f>R76/$N$77</f>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="15:18">
@@ -4871,17 +4868,17 @@
         <v>2</v>
       </c>
       <c r="Q78" s="63">
-        <f t="shared" si="0"/>
-        <v>1.25</v>
+        <f t="shared" ref="Q78:Q83" si="0">Q77/(P77*$N$77)</f>
+        <v>0.05</v>
       </c>
       <c r="R78" s="63">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f t="shared" ref="R77:R83" si="1">R77/$N$77</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="79" spans="7:18">
       <c r="G79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H79">
         <f>POWER(2,-2*$H$77)</f>
@@ -4893,16 +4890,16 @@
       </c>
       <c r="Q79" s="63">
         <f t="shared" si="0"/>
-        <v>0.208333333333333</v>
+        <v>0.0025</v>
       </c>
       <c r="R79" s="63">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="80" spans="7:18">
       <c r="G80" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H80">
         <v>10</v>
@@ -4913,16 +4910,16 @@
       </c>
       <c r="Q80" s="63">
         <f t="shared" si="0"/>
-        <v>0.0260416666666667</v>
+        <v>8.33333333333333e-5</v>
       </c>
       <c r="R80" s="63">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="81" spans="7:18">
       <c r="G81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H81">
         <f>H79*H80</f>
@@ -4934,11 +4931,11 @@
       </c>
       <c r="Q81" s="63">
         <f t="shared" si="0"/>
-        <v>0.00260416666666667</v>
+        <v>2.08333333333333e-6</v>
       </c>
       <c r="R81" s="63">
         <f t="shared" si="1"/>
-        <v>0.3125</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="82" spans="16:18">
@@ -4947,11 +4944,11 @@
       </c>
       <c r="Q82" s="63">
         <f t="shared" si="0"/>
-        <v>0.000217013888888889</v>
+        <v>4.16666666666667e-8</v>
       </c>
       <c r="R82" s="63">
         <f t="shared" si="1"/>
-        <v>0.15625</v>
+        <v>1e-5</v>
       </c>
     </row>
     <row r="83" spans="16:18">
@@ -4960,11 +4957,50 @@
       </c>
       <c r="Q83" s="63">
         <f t="shared" si="0"/>
-        <v>1.55009920634921e-5</v>
+        <v>6.94444444444444e-10</v>
       </c>
       <c r="R83" s="63">
         <f t="shared" si="1"/>
-        <v>0.078125</v>
+        <v>1e-6</v>
+      </c>
+    </row>
+    <row r="84" spans="16:18">
+      <c r="P84" s="63">
+        <v>8</v>
+      </c>
+      <c r="Q84" s="63">
+        <f>Q83/(P83*$N$77)</f>
+        <v>9.92063492063492e-12</v>
+      </c>
+      <c r="R84" s="63">
+        <f>R83/$N$77</f>
+        <v>1e-7</v>
+      </c>
+    </row>
+    <row r="85" spans="16:18">
+      <c r="P85" s="63">
+        <v>9</v>
+      </c>
+      <c r="Q85" s="63">
+        <f>Q84/(P84*$N$77)</f>
+        <v>1.24007936507937e-13</v>
+      </c>
+      <c r="R85" s="63">
+        <f>R84/$N$77</f>
+        <v>1e-8</v>
+      </c>
+    </row>
+    <row r="86" spans="16:18">
+      <c r="P86" s="63">
+        <v>10</v>
+      </c>
+      <c r="Q86" s="63">
+        <f>Q85/(P85*$N$77)</f>
+        <v>1.37786596119929e-15</v>
+      </c>
+      <c r="R86" s="63">
+        <f>R85/$N$77</f>
+        <v>1e-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>